<commit_message>
Adicionada a tabela Teams ao dicionário de dados do UML
</commit_message>
<xml_diff>
--- a/04 - Docs/01 - Project Manager/08 - UML/Dicionário Dados/Dicionário de dados.xlsx
+++ b/04 - Docs/01 - Project Manager/08 - UML/Dicionário Dados/Dicionário de dados.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\one\Desktop\Repos\WizBall\04 - Docs\01 - Project Manager\08 - UML\Dicionário Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userpo119pc16\Desktop\WizBall\04 - Docs\01 - Project Manager\08 - UML\Dicionário Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D083D62-25AA-4854-ABFF-E73CACB546E6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Matches" sheetId="1" r:id="rId1"/>
     <sheet name="Competitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Teams" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="88">
   <si>
     <t>MATCHES</t>
   </si>
@@ -236,12 +236,72 @@
   <si>
     <t>Data e hora que o registo da competição foi atualizada pela última vez.</t>
   </si>
+  <si>
+    <t>TEAMS</t>
+  </si>
+  <si>
+    <t>Nome completo da equipa.</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>Nome abreviado da equipa.</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Localização da sede da equipa.</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>Número de telefone da sede da equipa.</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>Site da equipa.</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email da sede da equipa.</t>
+  </si>
+  <si>
+    <t>founded</t>
+  </si>
+  <si>
+    <t>Ano de fundação da equipa.</t>
+  </si>
+  <si>
+    <t>club_colors</t>
+  </si>
+  <si>
+    <t>Cores principais da equipa.</t>
+  </si>
+  <si>
+    <t>venue</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>Nome do estádio da equipa.</t>
+  </si>
+  <si>
+    <t>Emblema da equipa.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +337,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -516,13 +582,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,54 +652,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,10 +661,19 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -908,11 +989,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,161 +1008,161 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="8">
-        <v>10</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="11">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="8">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>23</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="8">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9"/>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="8">
         <v>50</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="5">
         <v>50</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1090,264 +1171,264 @@
     </row>
     <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>23</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8">
-        <v>10</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="11">
-        <v>10</v>
-      </c>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="8">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="8">
-        <v>10</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="8">
         <v>50</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="11" t="s">
         <v>38</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="5">
         <v>50</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="12" t="s">
         <v>41</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="11">
-        <v>10</v>
-      </c>
-      <c r="F17" s="12" t="s">
+      <c r="D17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="8">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="8">
-        <v>10</v>
-      </c>
-      <c r="F18" s="9" t="s">
+      <c r="D18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="5">
+        <v>10</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="11">
-        <v>10</v>
-      </c>
-      <c r="F19" s="12" t="s">
+      <c r="D19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="8">
+        <v>10</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="8">
-        <v>10</v>
-      </c>
-      <c r="F20" s="9" t="s">
+      <c r="D20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="5">
+        <v>10</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="11">
-        <v>10</v>
-      </c>
-      <c r="F21" s="12" t="s">
+      <c r="D21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8">
+        <v>10</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="8">
-        <v>10</v>
-      </c>
-      <c r="F22" s="9" t="s">
+      <c r="D22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="5">
+        <v>10</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="11">
-        <v>10</v>
-      </c>
-      <c r="F23" s="12" t="s">
+      <c r="D23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="8">
+        <v>10</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="17">
-        <v>10</v>
-      </c>
-      <c r="F24" s="18" t="s">
+      <c r="D24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="14">
+        <v>10</v>
+      </c>
+      <c r="F24" s="15" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="3"/>
@@ -1369,11 +1450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A376DFF6-EF92-414F-B67C-C914A3E1B8D3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,123 +1469,123 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="21" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="8">
-        <v>10</v>
-      </c>
-      <c r="F4" s="9" t="s">
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="11">
-        <v>10</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="5">
         <v>50</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>50</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>66</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>23</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1530,4 +1611,273 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="5">
+        <v>50</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="8">
+        <v>50</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5">
+        <v>150</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="8">
+        <v>50</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="5">
+        <v>100</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="8">
+        <v>100</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="8">
+        <v>50</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="5">
+        <v>100</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="8">
+        <v>50</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="14">
+        <v>23</v>
+      </c>
+      <c r="F18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
actualização ao uml (modelo dados, fluxo de dados) e tabmbém aos scrips sql
</commit_message>
<xml_diff>
--- a/04 - Docs/01 - Project Manager/08 - UML/Dicionário Dados/Dicionário de dados.xlsx
+++ b/04 - Docs/01 - Project Manager/08 - UML/Dicionário Dados/Dicionário de dados.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\userpo119pc16\Desktop\WizBall\04 - Docs\01 - Project Manager\08 - UML\Dicionário Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\one\Desktop\Repos\WizBall\04 - Docs\01 - Project Manager\08 - UML\Dicionário Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBD950D-6367-410A-98B6-5035497C42F9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matches" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
   <si>
     <t>MATCHES</t>
   </si>
@@ -296,11 +297,14 @@
   <si>
     <t>Emblema da equipa.</t>
   </si>
+  <si>
+    <t>Número único utilizado para identificar o país da competição.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,6 +647,21 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -660,21 +679,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -989,10 +993,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1008,13 +1012,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1450,11 +1454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,13 +1473,13 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1614,15 +1618,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="73.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
@@ -1630,88 +1635,122 @@
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="32"/>
+    </row>
+    <row r="3" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>5</v>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="8">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>6</v>
+      <c r="B6" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>9</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E7" s="8">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
-        <v>62</v>
+      <c r="B8" s="23" t="s">
+        <v>72</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E8" s="5">
-        <v>50</v>
-      </c>
-      <c r="F8" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>23</v>
@@ -1724,17 +1763,17 @@
       </c>
     </row>
     <row r="10" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
-        <v>72</v>
+      <c r="B10" s="23" t="s">
+        <v>76</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="5">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>24</v>
@@ -1742,33 +1781,33 @@
     </row>
     <row r="11" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
-        <v>76</v>
+      <c r="B12" s="23" t="s">
+        <v>80</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E12" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>24</v>
@@ -1776,33 +1815,33 @@
     </row>
     <row r="13" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="8">
+        <v>50</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="5">
         <v>100</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="5">
-        <v>10</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>24</v>
@@ -1810,10 +1849,10 @@
     </row>
     <row r="15" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>23</v>
@@ -1825,58 +1864,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="5" t="s">
+    <row r="16" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="14">
         <v>23</v>
       </c>
-      <c r="E16" s="5">
-        <v>100</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="8">
-        <v>50</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="14">
-        <v>23</v>
-      </c>
-      <c r="F18" s="15"/>
+      <c r="F16" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>